<commit_message>
Files of properties added.
</commit_message>
<xml_diff>
--- a/back-end/arqsProjeto/modeloDeDados.xlsx
+++ b/back-end/arqsProjeto/modeloDeDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\NelioAlvesSpringBoot\BootCamp\zup\dsZupApostas\back-end\arqsProjeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3303BB4A-C0E3-4F4F-9063-3C562E0FB850}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF3E2D8-9FCB-47A2-B8E4-4E293196302A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{41A496F1-A057-452E-B1CF-2922E6F819F9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>tp_players</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Entregar como:</t>
+  </si>
+  <si>
+    <t>Mapeamento objeto-relacional</t>
   </si>
 </sst>
 </file>
@@ -176,11 +179,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -189,6 +189,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -504,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7883B6B3-67B4-4F09-A849-B9AFBF670D40}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,172 +526,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>19</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>3</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>42</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>61</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>52</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>37</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>73</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>81</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>84</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>19</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>86</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Com erro de listagem
</commit_message>
<xml_diff>
--- a/back-end/arqsProjeto/modeloDeDados.xlsx
+++ b/back-end/arqsProjeto/modeloDeDados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cursos\NelioAlvesSpringBoot\BootCamp\zup\dsZupApostas\back-end\arqsProjeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14B5630-831E-485F-BAF9-FBCFB7291EA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF7D376-12E2-4525-B52C-F164DFEF1026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{41A496F1-A057-452E-B1CF-2922E6F819F9}"/>
   </bookViews>
@@ -79,12 +79,6 @@
     <t>tb_players_apostas</t>
   </si>
   <si>
-    <t>id_players</t>
-  </si>
-  <si>
-    <t>id_apostas</t>
-  </si>
-  <si>
     <t>Para:</t>
   </si>
   <si>
@@ -113,6 +107,12 @@
   </si>
   <si>
     <t>Aqueiroga</t>
+  </si>
+  <si>
+    <t>players_id</t>
+  </si>
+  <si>
+    <t>apostas_id</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,16 +673,16 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="L8">
         <v>140</v>
@@ -770,39 +770,39 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>